<commit_message>
Merged PR 3434: PRI-6136: Import Diginet inventory template - Line Items (includes validation) BE
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/BarterDataFiles/Diginet_InvalidFile1.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/BarterDataFiles/Diginet_InvalidFile1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achyzh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\achyzh\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\BarterDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D361CAAF-5278-481B-8DCF-AA3BD91C127D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862321D8-546B-4FAA-B405-0F1A9A65F03D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Barter Header</t>
   </si>
@@ -71,16 +71,13 @@
     <t>HH Imps (000)</t>
   </si>
   <si>
-    <t>P 18-49 Rtg</t>
+    <t>Antenna TV</t>
   </si>
   <si>
-    <t>P 18-49 Imps (000)</t>
+    <t>F18-20 Rtg</t>
   </si>
   <si>
-    <t>M-F 6:00AM-8:00AM</t>
-  </si>
-  <si>
-    <t>Antenna TV</t>
+    <t>F18-20 Imps (000)</t>
   </si>
 </sst>
 </file>
@@ -1001,8 +998,8 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
@@ -1090,7 +1087,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>8</v>
@@ -1343,10 +1340,10 @@
         <v>13</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
@@ -1366,22 +1363,12 @@
       <c r="V11" s="15"/>
     </row>
     <row r="12" spans="1:26" ht="24" customHeight="1">
-      <c r="A12" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="A12" s="10"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="10">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="D12" s="10">
-        <v>158</v>
-      </c>
-      <c r="E12" s="10">
-        <v>0.06</v>
-      </c>
-      <c r="F12" s="10">
-        <v>77</v>
-      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="16"/>
       <c r="I12" s="10"/>

</xml_diff>